<commit_message>
added base schema for json added node-xlsx
</commit_message>
<xml_diff>
--- a/src/test2.xlsx
+++ b/src/test2.xlsx
@@ -71,9 +71,6 @@
     <t>offers[0].categoryId</t>
   </si>
   <si>
-    <t>currencies[0].id</t>
-  </si>
-  <si>
     <t>currencies[0].rate</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>modelname</t>
+  </si>
+  <si>
+    <t>currencies.id</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,10 +606,10 @@
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1" ht="47.25">
       <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -639,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>11</v>
@@ -651,19 +651,19 @@
         <v>14</v>
       </c>
       <c r="P1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="R1" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="8" customFormat="1" ht="300">
@@ -674,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -695,13 +695,13 @@
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1">
         <v>160</v>
@@ -710,22 +710,22 @@
         <v>13</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="17.25" customHeight="1"/>

</xml_diff>